<commit_message>
Report added, RunData updated, additional workbenches, lots of debugging
</commit_message>
<xml_diff>
--- a/runData.xlsx
+++ b/runData.xlsx
@@ -8,12 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolebarritt/Documents/CAB320/Spyder/CAB320-assignment1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41B1A6A9-9411-0447-A8BB-BB94B738399B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA439BC2-B958-7A47-9EEF-524FC76CA39C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16200" xr2:uid="{C7E23AAA-8D3A-204A-B611-3DF6F38CC543}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16200" activeTab="1" xr2:uid="{C7E23AAA-8D3A-204A-B611-3DF6F38CC543}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="AP1" sheetId="2" r:id="rId1"/>
+    <sheet name="AP2" sheetId="3" r:id="rId2"/>
+    <sheet name="AP3" sheetId="4" r:id="rId3"/>
+    <sheet name="AP4" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="21">
   <si>
     <t>ap</t>
   </si>
@@ -83,6 +86,12 @@
   <si>
     <t>DLS_5</t>
   </si>
+  <si>
+    <t>FOREVER</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
 </sst>
 </file>
 
@@ -91,7 +100,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -101,6 +110,14 @@
     </font>
     <font>
       <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -137,11 +154,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -458,8 +476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{940FB6CC-C773-3E47-A1AB-10193F1A9FCF}">
   <dimension ref="A1:K337"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView zoomScale="97" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1095,28 +1113,151 @@
       <c r="F18" t="s">
         <v>11</v>
       </c>
+      <c r="G18">
+        <v>1680.1410000000001</v>
+      </c>
+      <c r="H18">
+        <v>12802</v>
+      </c>
+      <c r="I18">
+        <v>12803</v>
+      </c>
+      <c r="J18">
+        <v>96446</v>
+      </c>
+      <c r="K18" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="19" spans="1:11">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19">
+        <v>9</v>
+      </c>
+      <c r="C19">
+        <v>9</v>
+      </c>
       <c r="D19" t="b">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
+      <c r="E19" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" t="s">
+        <v>12</v>
+      </c>
+      <c r="G19">
+        <v>4216.9539999999997</v>
+      </c>
+      <c r="H19">
+        <v>105192</v>
+      </c>
+      <c r="I19">
+        <v>105193</v>
+      </c>
+      <c r="J19">
+        <v>885099</v>
+      </c>
+      <c r="K19" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="20" spans="1:11">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20">
+        <v>9</v>
+      </c>
+      <c r="C20">
+        <v>9</v>
+      </c>
       <c r="D20" t="b">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
+      <c r="E20" t="s">
+        <v>15</v>
+      </c>
+      <c r="F20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G20" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="21" spans="1:11">
+      <c r="A21">
+        <v>1</v>
+      </c>
+      <c r="B21">
+        <v>9</v>
+      </c>
+      <c r="C21">
+        <v>9</v>
+      </c>
       <c r="D21" t="b">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
+      <c r="E21" t="s">
+        <v>17</v>
+      </c>
+      <c r="F21" t="s">
+        <v>16</v>
+      </c>
+      <c r="G21">
+        <v>147.26900000000001</v>
+      </c>
+      <c r="H21">
+        <v>28180</v>
+      </c>
+      <c r="I21">
+        <v>28181</v>
+      </c>
+      <c r="J21">
+        <v>28293</v>
+      </c>
+      <c r="K21" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="22" spans="1:11">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22">
+        <v>9</v>
+      </c>
+      <c r="C22">
+        <v>9</v>
+      </c>
       <c r="D22" t="b">
         <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E22" t="s">
+        <v>18</v>
+      </c>
+      <c r="F22" t="s">
+        <v>16</v>
+      </c>
+      <c r="G22">
+        <v>157.934</v>
+      </c>
+      <c r="H22">
+        <v>28180</v>
+      </c>
+      <c r="I22">
+        <v>28181</v>
+      </c>
+      <c r="J22">
+        <v>28393</v>
+      </c>
+      <c r="K22" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1180,97 +1321,100 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="4:4">
+    <row r="33" spans="4:5">
       <c r="D33" t="b">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="4:4">
+    <row r="34" spans="4:5">
       <c r="D34" t="b">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="4:4">
+    <row r="35" spans="4:5">
       <c r="D35" t="b">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="4:4">
+    <row r="36" spans="4:5">
       <c r="D36" t="b">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="4:4">
+    <row r="37" spans="4:5">
       <c r="D37" t="b">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="4:4">
+    <row r="38" spans="4:5">
       <c r="D38" t="b">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="4:4">
+      <c r="E38" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="39" spans="4:5">
       <c r="D39" t="b">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="4:4">
+    <row r="40" spans="4:5">
       <c r="D40" t="b">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="4:4">
+    <row r="41" spans="4:5">
       <c r="D41" t="b">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="4:4">
+    <row r="42" spans="4:5">
       <c r="D42" t="b">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="4:4">
+    <row r="43" spans="4:5">
       <c r="D43" t="b">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="4:4">
+    <row r="44" spans="4:5">
       <c r="D44" t="b">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="4:4">
+    <row r="45" spans="4:5">
       <c r="D45" t="b">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="4:4">
+    <row r="46" spans="4:5">
       <c r="D46" t="b">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="4:4">
+    <row r="47" spans="4:5">
       <c r="D47" t="b">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="4:4">
+    <row r="48" spans="4:5">
       <c r="D48" t="b">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -3014,4 +3158,1356 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{493DB849-5B2F-8F42-9EF7-0D6979D2F6A3}">
+  <dimension ref="A1:K58"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="1" spans="1:11" s="1" customFormat="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>5</v>
+      </c>
+      <c r="D2" t="b">
+        <f>IF(B2=C2,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2">
+        <v>0.84199999999999997</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
+      </c>
+      <c r="I2">
+        <v>3</v>
+      </c>
+      <c r="J2">
+        <v>3</v>
+      </c>
+      <c r="K2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>9</v>
+      </c>
+      <c r="C3">
+        <v>9</v>
+      </c>
+      <c r="D3" t="b">
+        <f t="shared" ref="D3:D58" si="0">IF(B3=C3,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3">
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="H3">
+        <v>4</v>
+      </c>
+      <c r="I3">
+        <v>5</v>
+      </c>
+      <c r="J3">
+        <v>11</v>
+      </c>
+      <c r="K3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>9</v>
+      </c>
+      <c r="C4">
+        <v>9</v>
+      </c>
+      <c r="D4" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4">
+        <v>0.111</v>
+      </c>
+      <c r="H4">
+        <v>4</v>
+      </c>
+      <c r="I4">
+        <v>5</v>
+      </c>
+      <c r="J4">
+        <v>11</v>
+      </c>
+      <c r="K4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>9</v>
+      </c>
+      <c r="C5">
+        <v>9</v>
+      </c>
+      <c r="D5" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5">
+        <v>0.499</v>
+      </c>
+      <c r="H5">
+        <v>54</v>
+      </c>
+      <c r="I5">
+        <v>55</v>
+      </c>
+      <c r="J5">
+        <v>77</v>
+      </c>
+      <c r="K5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>9</v>
+      </c>
+      <c r="C6">
+        <v>9</v>
+      </c>
+      <c r="D6" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6">
+        <v>0.33</v>
+      </c>
+      <c r="H6">
+        <v>20</v>
+      </c>
+      <c r="I6">
+        <v>21</v>
+      </c>
+      <c r="J6">
+        <v>42</v>
+      </c>
+      <c r="K6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>9</v>
+      </c>
+      <c r="C7">
+        <v>9</v>
+      </c>
+      <c r="D7" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7">
+        <v>0.34699999999999998</v>
+      </c>
+      <c r="H7">
+        <v>20</v>
+      </c>
+      <c r="I7">
+        <v>22</v>
+      </c>
+      <c r="J7">
+        <v>42</v>
+      </c>
+      <c r="K7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8">
+        <v>9</v>
+      </c>
+      <c r="C8">
+        <v>9</v>
+      </c>
+      <c r="D8" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8">
+        <v>0.10299999999999999</v>
+      </c>
+      <c r="H8">
+        <v>4</v>
+      </c>
+      <c r="I8">
+        <v>5</v>
+      </c>
+      <c r="J8">
+        <v>11</v>
+      </c>
+      <c r="K8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <v>5</v>
+      </c>
+      <c r="D9" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9">
+        <v>2.6440000000000002E-2</v>
+      </c>
+      <c r="H9">
+        <v>2</v>
+      </c>
+      <c r="I9">
+        <v>3</v>
+      </c>
+      <c r="J9">
+        <v>3</v>
+      </c>
+      <c r="K9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10">
+        <v>5</v>
+      </c>
+      <c r="C10">
+        <v>5</v>
+      </c>
+      <c r="D10" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="H10">
+        <v>2</v>
+      </c>
+      <c r="I10">
+        <v>3</v>
+      </c>
+      <c r="J10">
+        <v>3</v>
+      </c>
+      <c r="K10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11">
+        <v>5</v>
+      </c>
+      <c r="C11">
+        <v>5</v>
+      </c>
+      <c r="D11" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11">
+        <v>3.2300000000000002E-2</v>
+      </c>
+      <c r="H11">
+        <v>3</v>
+      </c>
+      <c r="I11">
+        <v>4</v>
+      </c>
+      <c r="J11">
+        <v>4</v>
+      </c>
+      <c r="K11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12">
+        <v>5</v>
+      </c>
+      <c r="C12">
+        <v>5</v>
+      </c>
+      <c r="D12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12">
+        <v>3.49E-2</v>
+      </c>
+      <c r="H12">
+        <v>3</v>
+      </c>
+      <c r="I12">
+        <v>4</v>
+      </c>
+      <c r="J12">
+        <v>4</v>
+      </c>
+      <c r="K12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="B13">
+        <v>5</v>
+      </c>
+      <c r="C13">
+        <v>5</v>
+      </c>
+      <c r="D13" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13">
+        <v>2.7699999999999999E-2</v>
+      </c>
+      <c r="H13">
+        <v>3</v>
+      </c>
+      <c r="I13" s="4">
+        <v>5</v>
+      </c>
+      <c r="J13">
+        <v>4</v>
+      </c>
+      <c r="K13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14">
+        <v>5</v>
+      </c>
+      <c r="C14">
+        <v>5</v>
+      </c>
+      <c r="D14" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F14" t="s">
+        <v>16</v>
+      </c>
+      <c r="G14">
+        <v>2.8899999999999999E-2</v>
+      </c>
+      <c r="H14">
+        <v>2</v>
+      </c>
+      <c r="I14">
+        <v>3</v>
+      </c>
+      <c r="J14">
+        <v>3</v>
+      </c>
+      <c r="K14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E15" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15">
+        <v>0.09</v>
+      </c>
+      <c r="H15">
+        <v>2</v>
+      </c>
+      <c r="I15">
+        <v>3</v>
+      </c>
+      <c r="J15">
+        <v>3</v>
+      </c>
+      <c r="K15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16">
+        <v>2</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" t="s">
+        <v>12</v>
+      </c>
+      <c r="G16">
+        <v>9.2700000000000005E-2</v>
+      </c>
+      <c r="H16">
+        <v>2</v>
+      </c>
+      <c r="I16">
+        <v>3</v>
+      </c>
+      <c r="J16">
+        <v>3</v>
+      </c>
+      <c r="K16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17">
+        <v>2</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E17" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" t="s">
+        <v>11</v>
+      </c>
+      <c r="G17">
+        <v>0.114</v>
+      </c>
+      <c r="H17">
+        <v>3</v>
+      </c>
+      <c r="I17">
+        <v>4</v>
+      </c>
+      <c r="J17">
+        <v>4</v>
+      </c>
+      <c r="K17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18">
+        <v>2</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" t="s">
+        <v>12</v>
+      </c>
+      <c r="G18">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="H18">
+        <v>3</v>
+      </c>
+      <c r="I18">
+        <v>4</v>
+      </c>
+      <c r="J18">
+        <v>4</v>
+      </c>
+      <c r="K18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19">
+        <v>2</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E19" t="s">
+        <v>15</v>
+      </c>
+      <c r="F19" t="s">
+        <v>11</v>
+      </c>
+      <c r="G19">
+        <v>0.121</v>
+      </c>
+      <c r="H19">
+        <v>3</v>
+      </c>
+      <c r="I19">
+        <v>5</v>
+      </c>
+      <c r="J19">
+        <v>4</v>
+      </c>
+      <c r="K19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20">
+        <v>2</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E20" t="s">
+        <v>17</v>
+      </c>
+      <c r="F20" t="s">
+        <v>16</v>
+      </c>
+      <c r="G20">
+        <v>0.107</v>
+      </c>
+      <c r="H20">
+        <v>2</v>
+      </c>
+      <c r="I20">
+        <v>3</v>
+      </c>
+      <c r="J20">
+        <v>3</v>
+      </c>
+      <c r="K20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21">
+        <v>2</v>
+      </c>
+      <c r="D21" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22">
+        <v>2</v>
+      </c>
+      <c r="D22" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="A23">
+        <v>2</v>
+      </c>
+      <c r="D23" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24">
+        <v>2</v>
+      </c>
+      <c r="D24" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
+      <c r="A25">
+        <v>2</v>
+      </c>
+      <c r="D25" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
+      <c r="A26">
+        <v>2</v>
+      </c>
+      <c r="D26" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
+      <c r="A27">
+        <v>2</v>
+      </c>
+      <c r="D27" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
+      <c r="A28">
+        <v>2</v>
+      </c>
+      <c r="D28" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
+      <c r="A29">
+        <v>2</v>
+      </c>
+      <c r="D29" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
+      <c r="A30">
+        <v>2</v>
+      </c>
+      <c r="D30" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11">
+      <c r="A31">
+        <v>2</v>
+      </c>
+      <c r="D31" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11">
+      <c r="A32">
+        <v>2</v>
+      </c>
+      <c r="D32" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33">
+        <v>2</v>
+      </c>
+      <c r="D33" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34">
+        <v>2</v>
+      </c>
+      <c r="D34" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35">
+        <v>2</v>
+      </c>
+      <c r="D35" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36">
+        <v>2</v>
+      </c>
+      <c r="D36" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37">
+        <v>2</v>
+      </c>
+      <c r="D37" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38">
+        <v>2</v>
+      </c>
+      <c r="D38" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39">
+        <v>2</v>
+      </c>
+      <c r="D39" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40">
+        <v>2</v>
+      </c>
+      <c r="D40" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41">
+        <v>2</v>
+      </c>
+      <c r="D41" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42">
+        <v>2</v>
+      </c>
+      <c r="D42" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="D43" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="D44" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="D45" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="D46" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="D47" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="D48" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="4:4">
+      <c r="D49" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="4:4">
+      <c r="D50" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="4:4">
+      <c r="D51" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="4:4">
+      <c r="D52" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="4:4">
+      <c r="D53" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="4:4">
+      <c r="D54" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="4:4">
+      <c r="D55" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="4:4">
+      <c r="D56" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="4:4">
+      <c r="D57" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="4:4">
+      <c r="D58" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E03A4F62-C48F-9044-A4D9-5441CEF830D7}">
+  <dimension ref="A1:K42"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="1" spans="1:11" s="1" customFormat="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="b">
+        <f>IF(B2=C2, TRUE, FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="D3" t="b">
+        <f t="shared" ref="D3:D42" si="0">IF(B3=C3, TRUE, FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="D4" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="D5" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="D6" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="D7" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="D8" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="D9" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="D10" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="D11" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="D12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="D13" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="D14" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="D15" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="D16" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4">
+      <c r="D17" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="4:4">
+      <c r="D18" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="4:4">
+      <c r="D19" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="4:4">
+      <c r="D20" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="4:4">
+      <c r="D21" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="4:4">
+      <c r="D22" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="4:4">
+      <c r="D23" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="4:4">
+      <c r="D24" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="4:4">
+      <c r="D25" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="4:4">
+      <c r="D26" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="4:4">
+      <c r="D27" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="4:4">
+      <c r="D28" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="4:4">
+      <c r="D29" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="4:4">
+      <c r="D30" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="4:4">
+      <c r="D31" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="4:4">
+      <c r="D32" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="4:4">
+      <c r="D33" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="4:4">
+      <c r="D34" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="4:4">
+      <c r="D35" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="4:4">
+      <c r="D36" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="4:4">
+      <c r="D37" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="4:4">
+      <c r="D38" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="4:4">
+      <c r="D39" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="4:4">
+      <c r="D40" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="4:4">
+      <c r="D41" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="4:4">
+      <c r="D42" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BA9A864-DF4C-534E-9418-62F462FF1816}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>